<commit_message>
feat: Update ciiu_2.0.xlsx and add new descripciones.xlsx file
</commit_message>
<xml_diff>
--- a/ciiu_2.0.xlsx
+++ b/ciiu_2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cpilla\Documents\DATA MANAGMENT\CIIU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\IdeaProjects\ciiu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCF7A44A-48B6-4AFC-9281-3E9213198207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F34177-617B-4DDE-82D7-5EA989A8602B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{52719EC8-DBE7-4793-AB7A-79F20E43DC71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{52719EC8-DBE7-4793-AB7A-79F20E43DC71}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16943,7 +16943,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -17262,10 +17262,10 @@
   <dimension ref="A1:F3058"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
     <col min="2" max="2" width="90.42578125" customWidth="1"/>
@@ -50869,7 +50869,7 @@
         <v>5578</v>
       </c>
       <c r="C3054" s="5" t="s">
-        <v>5592</v>
+        <v>5603</v>
       </c>
     </row>
     <row r="3055" spans="1:3" x14ac:dyDescent="0.25">
@@ -50880,7 +50880,7 @@
         <v>5580</v>
       </c>
       <c r="C3055" s="5" t="s">
-        <v>5592</v>
+        <v>5603</v>
       </c>
     </row>
     <row r="3056" spans="1:3" x14ac:dyDescent="0.25">
@@ -50891,7 +50891,7 @@
         <v>5582</v>
       </c>
       <c r="C3056" s="5" t="s">
-        <v>5592</v>
+        <v>5603</v>
       </c>
     </row>
     <row r="3057" spans="1:3" x14ac:dyDescent="0.25">
@@ -50902,7 +50902,7 @@
         <v>5584</v>
       </c>
       <c r="C3057" s="5" t="s">
-        <v>5592</v>
+        <v>5603</v>
       </c>
     </row>
     <row r="3058" spans="1:3" x14ac:dyDescent="0.25">
@@ -50913,7 +50913,7 @@
         <v>5586</v>
       </c>
       <c r="C3058" s="5" t="s">
-        <v>5592</v>
+        <v>5603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>